<commit_message>
Tweak starts and stops
Add a function to save specific onsets for confirming bell starts and
stops. Update xlsx with new starts and stops. Ignore .mp3 and .wav
files.
</commit_message>
<xml_diff>
--- a/bell_true_positives.xlsx
+++ b/bell_true_positives.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devin/Dropbox (Personal)/RotL Bells/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devin/Projects/rotl-bells/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -358,7 +358,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -395,7 +397,7 @@
         <v>rotl_0034</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>12.5</v>
       </c>
       <c r="D2">
         <v>13</v>
@@ -413,10 +415,10 @@
         <v>rotl_0034</v>
       </c>
       <c r="C3">
-        <v>16.5</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="D3">
-        <v>17.5</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -443,10 +445,10 @@
         <v>rotl_0034</v>
       </c>
       <c r="C5">
-        <v>1216</v>
+        <v>1216.44</v>
       </c>
       <c r="D5">
-        <v>1217</v>
+        <v>1217.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -458,10 +460,10 @@
         <v>rotl_0034</v>
       </c>
       <c r="C6">
-        <v>4996</v>
+        <v>4996.1000000000004</v>
       </c>
       <c r="D6">
-        <v>4997</v>
+        <v>4996.6000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>